<commit_message>
228.bin completed + title screen texture edited files
</commit_message>
<xml_diff>
--- a/misc/gnk_table.xlsx
+++ b/misc/gnk_table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ps2 stuff\C1GP_TranslationProject\C1_GP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ps2 stuff\C1GP_TranslationProject\RBC1GP-Translation-Pipeline\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="10830" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="char_table" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7502" uniqueCount="3681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7503" uniqueCount="3682">
   <si>
     <t>ぁ</t>
   </si>
@@ -11177,6 +11177,9 @@
   </si>
   <si>
     <t>special events data, fixed string length</t>
+  </si>
+  <si>
+    <t>useful regexp to find jp characters in vscode = [\u3040-\u309F\u30A0-\u30FF\u4E00-\u9FFF]</t>
   </si>
 </sst>
 </file>
@@ -12291,8 +12294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BN91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI31" sqref="BI31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15764,6 +15767,9 @@
       </c>
       <c r="BB26" s="36" t="s">
         <v>1401</v>
+      </c>
+      <c r="BD26" t="s">
+        <v>3681</v>
       </c>
     </row>
     <row r="27" spans="2:56">
@@ -25429,7 +25435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>